<commit_message>
Sprint en Product backlog
</commit_message>
<xml_diff>
--- a/documentatie/Product backlog overview & Sprint backlogs.xlsx
+++ b/documentatie/Product backlog overview & Sprint backlogs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6324" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6324"/>
   </bookViews>
   <sheets>
     <sheet name="PRODUCT BACKLOG" sheetId="1" r:id="rId1"/>
@@ -629,11 +629,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -15800,7 +15800,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -39065,7 +39065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>